<commit_message>
updated group form submission file
</commit_message>
<xml_diff>
--- a/Submission/GroupFormation/STA380GroupForm(Jeffrey, Faye).xlsx
+++ b/Submission/GroupFormation/STA380GroupForm(Jeffrey, Faye).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreyhuang/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD3B251A-3958-AD43-A804-EE29731C6868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE017291-ED60-B54C-80CC-198363F98DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>If left blank, you will be assigned a number.</t>
   </si>
@@ -97,9 +97,6 @@
     <t>HuangJeffrey</t>
   </si>
   <si>
-    <t>VaR calculator for stock portfolio through Monte Carlo</t>
-  </si>
-  <si>
     <t>https://github.com/HuangJeffrey/VaRMCProject.git</t>
   </si>
   <si>
@@ -110,6 +107,15 @@
   </si>
   <si>
     <t>sunjia89</t>
+  </si>
+  <si>
+    <t>VaR YYDS</t>
+  </si>
+  <si>
+    <t>VaR calculator for Stock Portfolio through Monte Carlo and Geometric Brownian Motion</t>
+  </si>
+  <si>
+    <t>https://github.com/fayeyeye</t>
   </si>
 </sst>
 </file>
@@ -408,8 +414,8 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -434,6 +440,9 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
@@ -448,7 +457,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -541,7 +550,7 @@
         <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -549,16 +558,19 @@
         <v>14</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22">
         <v>1009634941</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>